<commit_message>
built sql and python script builders, went back to work on match logic
</commit_message>
<xml_diff>
--- a/Column rename and reorder interface.xlsx
+++ b/Column rename and reorder interface.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpiston\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danpiston/Documents/code/column-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8DF698-F73C-4821-AAE0-7B34BE4D7618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BCA7D1-010D-8341-B7C4-B51974C71BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBAD64F4-91D6-4D09-B42B-90199B83CC82}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{FBAD64F4-91D6-4D09-B42B-90199B83CC82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1055,12 +1055,12 @@
   <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1106,7 +1106,7 @@
       <c r="AJ2" s="4"/>
       <c r="AK2" s="5"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="AK3" s="9"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14"/>
@@ -1192,7 +1192,7 @@
       <c r="AJ4" s="8"/>
       <c r="AK4" s="9"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="AK5" s="9"/>
     </row>
-    <row r="6" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
         <v>3</v>
@@ -1276,7 +1276,7 @@
       <c r="AJ6" s="8"/>
       <c r="AK6" s="9"/>
     </row>
-    <row r="7" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="AK7" s="9"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1360,7 +1360,7 @@
       <c r="AJ8" s="8"/>
       <c r="AK8" s="9"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
         <v>26</v>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="AK9" s="9"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -1442,7 +1442,7 @@
       <c r="AJ10" s="8"/>
       <c r="AK10" s="9"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1479,7 +1479,7 @@
       <c r="AJ11" s="8"/>
       <c r="AK11" s="9"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1516,7 +1516,7 @@
       <c r="AJ12" s="8"/>
       <c r="AK12" s="9"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1551,7 +1551,7 @@
       <c r="AJ13" s="11"/>
       <c r="AK13" s="12"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="N14" s="6"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
@@ -1564,7 +1564,7 @@
       <c r="W14" s="8"/>
       <c r="X14" s="9"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="9"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1604,7 +1604,7 @@
       <c r="W16" s="8"/>
       <c r="X16" s="9"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="8"/>
       <c r="C17" s="17" t="s">
@@ -1613,10 +1613,10 @@
       <c r="D17" s="17"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="9"/>
@@ -1636,7 +1636,7 @@
       <c r="W17" s="8"/>
       <c r="X17" s="9"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1660,7 +1660,7 @@
       <c r="W18" s="8"/>
       <c r="X18" s="9"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="8"/>
       <c r="C19" s="18" t="s">
@@ -1688,7 +1688,7 @@
       <c r="W19" s="11"/>
       <c r="X19" s="12"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1701,7 +1701,7 @@
       <c r="J20" s="8"/>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="8"/>
       <c r="C21" s="18" t="s">
@@ -1718,7 +1718,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1734,7 +1734,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="8"/>
       <c r="C23" s="18" t="s">
@@ -1756,7 +1756,7 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="39"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1776,7 +1776,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="41"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="8"/>
       <c r="C25" s="18" t="s">
@@ -1800,7 +1800,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="41"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1818,7 +1818,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="41"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="8"/>
       <c r="C27" s="18" t="s">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="Q27" s="41"/>
     </row>
-    <row r="28" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1862,7 +1862,7 @@
       <c r="P28" s="44"/>
       <c r="Q28" s="45"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="8"/>
       <c r="C29" s="18" t="s">
@@ -1877,7 +1877,7 @@
       <c r="J29" s="8"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1890,7 +1890,7 @@
       <c r="J30" s="8"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1907,7 +1907,7 @@
       <c r="J31" s="8"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1920,7 +1920,7 @@
       <c r="J32" s="8"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>

</xml_diff>

<commit_message>
cleaned up script screen and worked on match screen button logic
</commit_message>
<xml_diff>
--- a/Column rename and reorder interface.xlsx
+++ b/Column rename and reorder interface.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danpiston/Documents/code/column-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BCA7D1-010D-8341-B7C4-B51974C71BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD7EF8B-395A-1142-A38A-A5702E691A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{FBAD64F4-91D6-4D09-B42B-90199B83CC82}"/>
+    <workbookView xWindow="0" yWindow="1720" windowWidth="23260" windowHeight="12580" xr2:uid="{FBAD64F4-91D6-4D09-B42B-90199B83CC82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Screen 1:</t>
   </si>
@@ -163,6 +164,75 @@
   </si>
   <si>
     <t>error between screen2 and screen3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t </t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>sun</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>why</t>
+  </si>
+  <si>
+    <t>1 hr of interview questions, dogs, target, eat dinner, 8 oclcock</t>
+  </si>
+  <si>
+    <t>prior:</t>
+  </si>
+  <si>
+    <t>counseling pm, brain felt tired, general malaise towards work</t>
+  </si>
+  <si>
+    <t>-button color with bootstrap?</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>weird zoom schedule and burned the fuck out, 1 hr of interview questions, Buckley/house stress</t>
+  </si>
+  <si>
+    <t>shots, mice people late, prep for parents here</t>
+  </si>
+  <si>
+    <t>parents here</t>
+  </si>
+  <si>
+    <t>micah home, up at 3:30 and exhausted from parents here</t>
   </si>
 </sst>
 </file>
@@ -482,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -529,6 +599,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CA8BD5-A145-41BE-A416-9F1886B31D96}">
-  <dimension ref="A1:AK33"/>
+  <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="L8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1701,7 @@
       <c r="R17" s="23"/>
       <c r="S17" s="8"/>
       <c r="T17" s="24" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
@@ -1717,6 +1789,13 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="9"/>
+      <c r="U21" t="s">
+        <v>55</v>
+      </c>
+      <c r="W21">
+        <f>0.5+0.5+0.5+1+1.25+1.75+1.25+1+0.25+1</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
@@ -1733,6 +1812,15 @@
       <c r="M22" t="s">
         <v>42</v>
       </c>
+      <c r="V22" t="s">
+        <v>51</v>
+      </c>
+      <c r="W22" t="s">
+        <v>52</v>
+      </c>
+      <c r="X22" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
@@ -1755,6 +1843,18 @@
       <c r="O23" s="38"/>
       <c r="P23" s="38"/>
       <c r="Q23" s="39"/>
+      <c r="U23" t="s">
+        <v>43</v>
+      </c>
+      <c r="V23">
+        <v>2</v>
+      </c>
+      <c r="W23">
+        <v>1.25</v>
+      </c>
+      <c r="X23" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
@@ -1775,6 +1875,18 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="41"/>
+      <c r="U24" t="s">
+        <v>44</v>
+      </c>
+      <c r="V24">
+        <v>4</v>
+      </c>
+      <c r="W24" s="47">
+        <v>3.25</v>
+      </c>
+      <c r="X24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
@@ -1799,6 +1911,18 @@
       <c r="O25" s="42"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="41"/>
+      <c r="U25" t="s">
+        <v>45</v>
+      </c>
+      <c r="V25">
+        <v>4</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
@@ -1817,6 +1941,18 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="41"/>
+      <c r="U26" t="s">
+        <v>46</v>
+      </c>
+      <c r="V26">
+        <v>2</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
@@ -1843,6 +1979,18 @@
         <v>32</v>
       </c>
       <c r="Q27" s="41"/>
+      <c r="U27" t="s">
+        <v>47</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="28" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
@@ -1861,6 +2009,18 @@
       <c r="O28" s="44"/>
       <c r="P28" s="44"/>
       <c r="Q28" s="45"/>
+      <c r="U28" t="s">
+        <v>48</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
@@ -1876,6 +2036,18 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="9"/>
+      <c r="U29" t="s">
+        <v>49</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <v>2</v>
+      </c>
+      <c r="X29" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
@@ -1889,6 +2061,12 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="9"/>
+      <c r="U30" t="s">
+        <v>43</v>
+      </c>
+      <c r="V30">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
@@ -1906,6 +2084,12 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="9"/>
+      <c r="U31" t="s">
+        <v>44</v>
+      </c>
+      <c r="V31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
@@ -1919,8 +2103,14 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="U32" t="s">
+        <v>45</v>
+      </c>
+      <c r="V32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -1932,10 +2122,101 @@
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="12"/>
+      <c r="U33" t="s">
+        <v>46</v>
+      </c>
+      <c r="V33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M34" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="U34" t="s">
+        <v>47</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U35" t="s">
+        <v>48</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U36" t="s">
+        <v>49</v>
+      </c>
+      <c r="V36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U37" t="s">
+        <v>50</v>
+      </c>
+      <c r="V37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U38" t="s">
+        <v>44</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V39">
+        <f>SUM(V23:V38)</f>
+        <v>33</v>
+      </c>
+      <c r="W39">
+        <f>SUM(W23:W38)</f>
+        <v>6.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87586534-6129-7C49-87BB-08BD02D0CCF6}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
got state working through all three main frontend components
</commit_message>
<xml_diff>
--- a/Column rename and reorder interface.xlsx
+++ b/Column rename and reorder interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danpiston/Documents/code/column-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0E2BED-8E7A-EA44-B176-5A9C7E6D2236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBB378D-3B3B-8146-B4E3-1D539D1B6868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1720" windowWidth="23260" windowHeight="12580" xr2:uid="{FBAD64F4-91D6-4D09-B42B-90199B83CC82}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>Screen 1:</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>micah home, up at 3:30 and exhausted from parents here, mice people here</t>
+  </si>
+  <si>
+    <t>nothing to do at work, will need to run to target and have counseling later</t>
   </si>
 </sst>
 </file>
@@ -264,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +304,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -552,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -601,6 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1124,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CA8BD5-A145-41BE-A416-9F1886B31D96}">
-  <dimension ref="A1:AK39"/>
+  <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="J10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2067,6 +2077,12 @@
       <c r="V30">
         <v>3</v>
       </c>
+      <c r="W30">
+        <v>3</v>
+      </c>
+      <c r="X30" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
@@ -2179,7 +2195,13 @@
       </c>
       <c r="W39">
         <f>SUM(W23:W38)</f>
-        <v>6.5</v>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W40" s="48">
+        <f>W21+W39</f>
+        <v>18.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>